<commit_message>
Changed the default email address(sender). Added exception handling in new.html.erb. Also removed some unnecessary spaces and comments.
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/"CaÃ±ete","Carol Ann".xlsx
+++ b/exceltocsv/public/reports/employee dtr/"CaÃ±ete","Carol Ann".xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="67" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="67" xml:space="preserve">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -613,130 +613,138 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P7" s="5" t="inlineStr">
+      <c r="D7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P7" s="7" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P8" s="5" t="inlineStr">
+      <c r="D8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P8" s="7" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P9" s="5" t="inlineStr">
+      <c r="D9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P9" s="7" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="n">
+      <c r="D10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7" t="n">
         <v>0.25</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P10" s="5" t="inlineStr">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P10" s="7" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -831,170 +839,180 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="n">
+      <c r="D14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P14" s="5" t="inlineStr">
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P14" s="7" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="n">
+      <c r="D15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P15" s="5" t="inlineStr">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P15" s="7" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="n">
+      <c r="D16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="7" t="n">
         <v>0.75</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P16" s="5" t="inlineStr">
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P16" s="7" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="n">
+      <c r="D17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="7" t="n">
         <v>1.0</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P17" s="5" t="inlineStr">
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P17" s="7" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="n">
+      <c r="D18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P18" s="5" t="inlineStr">
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P18" s="7" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>